<commit_message>
Finished changes Aug 12
</commit_message>
<xml_diff>
--- a/data_aug4/SO-PackExport Data_1011854_override.xlsx
+++ b/data_aug4/SO-PackExport Data_1011854_override.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\McRae\Source\bundle-optimization-new\data_aug4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\braedonm\source\bundle-optimization\data_aug4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7EA109B5-1495-4DB1-862A-7331ED6C01EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A234A7-8DF4-4231-88CA-4BB7BC91955A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SO-PackExportData" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="80">
   <si>
     <t>OrderType</t>
   </si>
@@ -260,9 +260,6 @@
   </si>
   <si>
     <t>HITCH Standard 0.75" Girt - 192" - Per Piece</t>
-  </si>
-  <si>
-    <t>x</t>
   </si>
 </sst>
 </file>
@@ -303,12 +300,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -531,7 +525,7 @@
   <dimension ref="A1:AP12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -707,122 +701,122 @@
       </c>
     </row>
     <row r="2" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="2">
-        <v>1011854</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1011854</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>15</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="2" t="s">
+      <c r="F2" s="1"/>
+      <c r="G2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="J2" s="2" t="s">
+      <c r="H2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="K2" s="3"/>
-      <c r="L2" s="2" t="s">
+      <c r="K2" s="1"/>
+      <c r="L2" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="O2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="P2" s="4">
-        <v>45712</v>
-      </c>
-      <c r="Q2" s="4">
-        <v>45712</v>
-      </c>
-      <c r="R2" s="4">
-        <v>45712</v>
-      </c>
-      <c r="S2" s="3"/>
-      <c r="T2" s="5"/>
-      <c r="U2" s="2">
+      <c r="P2" s="2">
+        <v>45712</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>45712</v>
+      </c>
+      <c r="R2" s="2">
+        <v>45712</v>
+      </c>
+      <c r="S2" s="1"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="1">
         <v>7509365</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="V2" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="W2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="X2" s="4">
+      <c r="X2" s="2">
         <v>81895</v>
       </c>
-      <c r="Y2" s="4">
+      <c r="Y2" s="2">
         <v>45721.70669475694</v>
       </c>
-      <c r="Z2" s="2">
+      <c r="Z2" s="1">
         <v>160</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AA2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AB2" s="2">
+      <c r="AB2" s="1">
         <v>2.9029889999999998</v>
       </c>
-      <c r="AC2" s="2">
+      <c r="AC2" s="1">
         <v>6.4</v>
       </c>
-      <c r="AD2" s="2">
+      <c r="AD2" s="1">
         <v>120</v>
       </c>
-      <c r="AE2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AF2" s="2">
-        <v>1011854</v>
-      </c>
-      <c r="AG2" s="2">
+      <c r="AE2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF2" s="1">
+        <v>1011854</v>
+      </c>
+      <c r="AG2" s="1">
         <v>1</v>
       </c>
-      <c r="AH2" s="2">
+      <c r="AH2" s="1">
         <v>30530</v>
       </c>
-      <c r="AI2" s="2">
+      <c r="AI2" s="1">
         <v>25523</v>
       </c>
-      <c r="AJ2" s="2" t="s">
+      <c r="AJ2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AK2" s="2" t="s">
+      <c r="AK2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AL2" s="2" t="s">
+      <c r="AL2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AM2" s="2" t="s">
+      <c r="AM2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AN2" s="2" t="s">
+      <c r="AN2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AO2" s="2">
+      <c r="AO2" s="1">
         <v>63177</v>
       </c>
-      <c r="AP2" s="2" t="s">
+      <c r="AP2" s="1" t="s">
         <v>50</v>
       </c>
     </row>
@@ -830,21 +824,19 @@
       <c r="A3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>1011854</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>80</v>
-      </c>
+      <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
         <v>54</v>
       </c>
@@ -857,7 +849,7 @@
       <c r="J3" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="K3" s="3"/>
+      <c r="K3" s="1"/>
       <c r="L3" s="1" t="s">
         <v>69</v>
       </c>
@@ -870,17 +862,17 @@
       <c r="O3" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="P3" s="4">
-        <v>45712</v>
-      </c>
-      <c r="Q3" s="4">
-        <v>45712</v>
-      </c>
-      <c r="R3" s="4">
-        <v>45712</v>
-      </c>
-      <c r="S3" s="3"/>
-      <c r="T3" s="5"/>
+      <c r="P3" s="2">
+        <v>45712</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>45712</v>
+      </c>
+      <c r="R3" s="2">
+        <v>45712</v>
+      </c>
+      <c r="S3" s="1"/>
+      <c r="T3" s="2"/>
       <c r="U3" s="1">
         <v>7509365</v>
       </c>
@@ -890,10 +882,10 @@
       <c r="W3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="X3" s="4">
+      <c r="X3" s="2">
         <v>81895</v>
       </c>
-      <c r="Y3" s="4">
+      <c r="Y3" s="2">
         <v>45721.70669475694</v>
       </c>
       <c r="Z3" s="1">
@@ -952,19 +944,19 @@
       <c r="A4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>1011854</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>20</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F4" s="3"/>
+      <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
         <v>73</v>
       </c>
@@ -977,7 +969,7 @@
       <c r="J4" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="K4" s="3"/>
+      <c r="K4" s="1"/>
       <c r="L4" s="1" t="s">
         <v>69</v>
       </c>
@@ -990,17 +982,17 @@
       <c r="O4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="P4" s="4">
-        <v>45712</v>
-      </c>
-      <c r="Q4" s="4">
-        <v>45712</v>
-      </c>
-      <c r="R4" s="4">
-        <v>45712</v>
-      </c>
-      <c r="S4" s="3"/>
-      <c r="T4" s="5"/>
+      <c r="P4" s="2">
+        <v>45712</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>45712</v>
+      </c>
+      <c r="R4" s="2">
+        <v>45712</v>
+      </c>
+      <c r="S4" s="1"/>
+      <c r="T4" s="2"/>
       <c r="U4" s="1">
         <v>7509365</v>
       </c>
@@ -1010,10 +1002,10 @@
       <c r="W4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="X4" s="4">
+      <c r="X4" s="2">
         <v>81895</v>
       </c>
-      <c r="Y4" s="4">
+      <c r="Y4" s="2">
         <v>45721.70669475694</v>
       </c>
       <c r="Z4" s="1">
@@ -1072,21 +1064,19 @@
       <c r="A5" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>1011854</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>5</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>80</v>
-      </c>
+      <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
         <v>64</v>
       </c>
@@ -1099,7 +1089,7 @@
       <c r="J5" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="K5" s="3"/>
+      <c r="K5" s="1"/>
       <c r="L5" s="1" t="s">
         <v>69</v>
       </c>
@@ -1112,17 +1102,17 @@
       <c r="O5" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="P5" s="4">
-        <v>45712</v>
-      </c>
-      <c r="Q5" s="4">
-        <v>45712</v>
-      </c>
-      <c r="R5" s="4">
-        <v>45712</v>
-      </c>
-      <c r="S5" s="3"/>
-      <c r="T5" s="5"/>
+      <c r="P5" s="2">
+        <v>45712</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>45712</v>
+      </c>
+      <c r="R5" s="2">
+        <v>45712</v>
+      </c>
+      <c r="S5" s="1"/>
+      <c r="T5" s="2"/>
       <c r="U5" s="1">
         <v>7509365</v>
       </c>
@@ -1132,10 +1122,10 @@
       <c r="W5" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="X5" s="4">
+      <c r="X5" s="2">
         <v>81895</v>
       </c>
-      <c r="Y5" s="4">
+      <c r="Y5" s="2">
         <v>45721.70669475694</v>
       </c>
       <c r="Z5" s="1">
@@ -1194,21 +1184,19 @@
       <c r="A6" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>1011854</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>5</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>80</v>
-      </c>
+      <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
         <v>56</v>
       </c>
@@ -1221,7 +1209,7 @@
       <c r="J6" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="K6" s="3"/>
+      <c r="K6" s="1"/>
       <c r="L6" s="1" t="s">
         <v>69</v>
       </c>
@@ -1234,17 +1222,17 @@
       <c r="O6" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="P6" s="4">
-        <v>45712</v>
-      </c>
-      <c r="Q6" s="4">
-        <v>45712</v>
-      </c>
-      <c r="R6" s="4">
-        <v>45712</v>
-      </c>
-      <c r="S6" s="3"/>
-      <c r="T6" s="5"/>
+      <c r="P6" s="2">
+        <v>45712</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>45712</v>
+      </c>
+      <c r="R6" s="2">
+        <v>45712</v>
+      </c>
+      <c r="S6" s="1"/>
+      <c r="T6" s="2"/>
       <c r="U6" s="1">
         <v>7509365</v>
       </c>
@@ -1254,10 +1242,10 @@
       <c r="W6" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="X6" s="4">
+      <c r="X6" s="2">
         <v>81895</v>
       </c>
-      <c r="Y6" s="4">
+      <c r="Y6" s="2">
         <v>45721.70669475694</v>
       </c>
       <c r="Z6" s="1">
@@ -1316,19 +1304,19 @@
       <c r="A7" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>1011854</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>5</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F7" s="3"/>
+      <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
         <v>66</v>
       </c>
@@ -1341,7 +1329,7 @@
       <c r="J7" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="K7" s="3"/>
+      <c r="K7" s="1"/>
       <c r="L7" s="1" t="s">
         <v>69</v>
       </c>
@@ -1354,17 +1342,17 @@
       <c r="O7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="P7" s="4">
-        <v>45712</v>
-      </c>
-      <c r="Q7" s="4">
-        <v>45712</v>
-      </c>
-      <c r="R7" s="4">
-        <v>45712</v>
-      </c>
-      <c r="S7" s="3"/>
-      <c r="T7" s="5"/>
+      <c r="P7" s="2">
+        <v>45712</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>45712</v>
+      </c>
+      <c r="R7" s="2">
+        <v>45712</v>
+      </c>
+      <c r="S7" s="1"/>
+      <c r="T7" s="2"/>
       <c r="U7" s="1">
         <v>7509365</v>
       </c>
@@ -1374,10 +1362,10 @@
       <c r="W7" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="X7" s="4">
+      <c r="X7" s="2">
         <v>81895</v>
       </c>
-      <c r="Y7" s="4">
+      <c r="Y7" s="2">
         <v>45721.70669475694</v>
       </c>
       <c r="Z7" s="1">
@@ -1436,19 +1424,19 @@
       <c r="A8" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>1011854</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="1">
         <v>5</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F8" s="3"/>
+      <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
         <v>58</v>
       </c>
@@ -1461,7 +1449,7 @@
       <c r="J8" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="K8" s="3"/>
+      <c r="K8" s="1"/>
       <c r="L8" s="1" t="s">
         <v>69</v>
       </c>
@@ -1474,17 +1462,17 @@
       <c r="O8" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="P8" s="4">
-        <v>45712</v>
-      </c>
-      <c r="Q8" s="4">
-        <v>45712</v>
-      </c>
-      <c r="R8" s="4">
-        <v>45712</v>
-      </c>
-      <c r="S8" s="3"/>
-      <c r="T8" s="5"/>
+      <c r="P8" s="2">
+        <v>45712</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>45712</v>
+      </c>
+      <c r="R8" s="2">
+        <v>45712</v>
+      </c>
+      <c r="S8" s="1"/>
+      <c r="T8" s="2"/>
       <c r="U8" s="1">
         <v>7509365</v>
       </c>
@@ -1494,10 +1482,10 @@
       <c r="W8" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="X8" s="4">
+      <c r="X8" s="2">
         <v>81895</v>
       </c>
-      <c r="Y8" s="4">
+      <c r="Y8" s="2">
         <v>45721.70669475694</v>
       </c>
       <c r="Z8" s="1">
@@ -1556,19 +1544,19 @@
       <c r="A9" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>1011854</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1">
         <v>5</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F9" s="3"/>
+      <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
         <v>60</v>
       </c>
@@ -1581,7 +1569,7 @@
       <c r="J9" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="K9" s="3"/>
+      <c r="K9" s="1"/>
       <c r="L9" s="1" t="s">
         <v>69</v>
       </c>
@@ -1594,17 +1582,17 @@
       <c r="O9" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="P9" s="4">
-        <v>45712</v>
-      </c>
-      <c r="Q9" s="4">
-        <v>45712</v>
-      </c>
-      <c r="R9" s="4">
-        <v>45712</v>
-      </c>
-      <c r="S9" s="3"/>
-      <c r="T9" s="5"/>
+      <c r="P9" s="2">
+        <v>45712</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>45712</v>
+      </c>
+      <c r="R9" s="2">
+        <v>45712</v>
+      </c>
+      <c r="S9" s="1"/>
+      <c r="T9" s="2"/>
       <c r="U9" s="1">
         <v>7509365</v>
       </c>
@@ -1614,10 +1602,10 @@
       <c r="W9" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="X9" s="4">
+      <c r="X9" s="2">
         <v>81895</v>
       </c>
-      <c r="Y9" s="4">
+      <c r="Y9" s="2">
         <v>45721.70669475694</v>
       </c>
       <c r="Z9" s="1">
@@ -1676,19 +1664,19 @@
       <c r="A10" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>1011854</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="1">
         <v>50</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F10" s="3"/>
+      <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
         <v>75</v>
       </c>
@@ -1701,7 +1689,7 @@
       <c r="J10" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="K10" s="3"/>
+      <c r="K10" s="1"/>
       <c r="L10" s="1" t="s">
         <v>69</v>
       </c>
@@ -1714,17 +1702,17 @@
       <c r="O10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="P10" s="4">
-        <v>45712</v>
-      </c>
-      <c r="Q10" s="4">
-        <v>45712</v>
-      </c>
-      <c r="R10" s="4">
-        <v>45712</v>
-      </c>
-      <c r="S10" s="3"/>
-      <c r="T10" s="5"/>
+      <c r="P10" s="2">
+        <v>45712</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>45712</v>
+      </c>
+      <c r="R10" s="2">
+        <v>45712</v>
+      </c>
+      <c r="S10" s="1"/>
+      <c r="T10" s="2"/>
       <c r="U10" s="1">
         <v>7509365</v>
       </c>
@@ -1734,10 +1722,10 @@
       <c r="W10" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="X10" s="4">
+      <c r="X10" s="2">
         <v>81895</v>
       </c>
-      <c r="Y10" s="4">
+      <c r="Y10" s="2">
         <v>45721.70669475694</v>
       </c>
       <c r="Z10" s="1">
@@ -1796,19 +1784,19 @@
       <c r="A11" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>1011854</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="1">
         <v>17</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F11" s="3"/>
+      <c r="F11" s="1"/>
       <c r="G11" s="1" t="s">
         <v>77</v>
       </c>
@@ -1821,7 +1809,7 @@
       <c r="J11" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="K11" s="3"/>
+      <c r="K11" s="1"/>
       <c r="L11" s="1" t="s">
         <v>69</v>
       </c>
@@ -1834,17 +1822,17 @@
       <c r="O11" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="P11" s="4">
-        <v>45712</v>
-      </c>
-      <c r="Q11" s="4">
-        <v>45712</v>
-      </c>
-      <c r="R11" s="4">
-        <v>45712</v>
-      </c>
-      <c r="S11" s="3"/>
-      <c r="T11" s="3"/>
+      <c r="P11" s="2">
+        <v>45712</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>45712</v>
+      </c>
+      <c r="R11" s="2">
+        <v>45712</v>
+      </c>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
       <c r="U11" s="1">
         <v>7509365</v>
       </c>
@@ -1854,10 +1842,10 @@
       <c r="W11" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="X11" s="4">
+      <c r="X11" s="2">
         <v>81895</v>
       </c>
-      <c r="Y11" s="4">
+      <c r="Y11" s="2">
         <v>45721.70669475694</v>
       </c>
       <c r="Z11" s="1">
@@ -1916,19 +1904,19 @@
       <c r="A12" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>1011854</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="1">
         <v>35</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F12" s="3"/>
+      <c r="F12" s="1"/>
       <c r="G12" s="1" t="s">
         <v>79</v>
       </c>
@@ -1941,7 +1929,7 @@
       <c r="J12" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="K12" s="3"/>
+      <c r="K12" s="1"/>
       <c r="L12" s="1" t="s">
         <v>69</v>
       </c>
@@ -1954,17 +1942,17 @@
       <c r="O12" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="P12" s="4">
-        <v>45712</v>
-      </c>
-      <c r="Q12" s="4">
-        <v>45712</v>
-      </c>
-      <c r="R12" s="4">
-        <v>45712</v>
-      </c>
-      <c r="S12" s="3"/>
-      <c r="T12" s="3"/>
+      <c r="P12" s="2">
+        <v>45712</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>45712</v>
+      </c>
+      <c r="R12" s="2">
+        <v>45712</v>
+      </c>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
       <c r="U12" s="1">
         <v>7509365</v>
       </c>
@@ -1974,10 +1962,10 @@
       <c r="W12" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="X12" s="4">
+      <c r="X12" s="2">
         <v>81895</v>
       </c>
-      <c r="Y12" s="4">
+      <c r="Y12" s="2">
         <v>45721.70669475694</v>
       </c>
       <c r="Z12" s="1">

</xml_diff>